<commit_message>
-added img in .docx -added rules.txt
</commit_message>
<xml_diff>
--- a/CheckFold/data.xlsx
+++ b/CheckFold/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="38">
   <si>
     <t xml:space="preserve">TaskNum</t>
   </si>
@@ -85,52 +85,55 @@
     <t xml:space="preserve">---</t>
   </si>
   <si>
+    <t xml:space="preserve">1.jpg,2.jpg,3.jpg, _3.jpg, 4.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20160802/3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Девять (8) изображений</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Письменного стола "Триан-41"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Белый, Белый-Дуб сонома, Венге, Венге-Дуб молочный, Венге-Дуб сонома, Дуб молочный-Венге, Дуб сонома-Белый, Дуб сонома-Венге</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.jpg,2.jpg,3.jpg,4.jpg,1.jpg,2.jpg,3.jpg,4.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20160802/4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Девять (9) изображений</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Письменного стола "Триан-42"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Дуб сонома-Белый</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.jpg,2.jpg,3.jpg,4.jpg,1.jpg,2.jpg,3.jpg,4.jpg,1.jpg,2.jpg,3.jpg,4.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20160802/5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Девять (10) изображений</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Письменного стола "Триан-43"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Белый-Дуб сонома</t>
+  </si>
+  <si>
+    <t xml:space="preserve">main.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">1.jpg,2.jpg,3.jpg,4.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20160802/3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Девять (8) изображений</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Письменного стола "Триан-41"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Белый, Белый-Дуб сонома, Венге, Венге-Дуб молочный, Венге-Дуб сонома, Дуб молочный-Венге, Дуб сонома-Белый, Дуб сонома-Венге</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.jpg,2.jpg,3.jpg,4.jpg,1.jpg,2.jpg,3.jpg,4.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20160802/4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Девять (9) изображений</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Письменного стола "Триан-42"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Дуб сонома-Белый</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.jpg,2.jpg,3.jpg,4.jpg,1.jpg,2.jpg,3.jpg,4.jpg,1.jpg,2.jpg,3.jpg,4.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20160802/5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Девять (10) изображений</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Письменного стола "Триан-43"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Белый-Дуб сонома</t>
-  </si>
-  <si>
-    <t xml:space="preserve">main.jpg</t>
   </si>
 </sst>
 </file>
@@ -235,7 +238,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -416,7 +419,7 @@
         <v>36</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>